<commit_message>
First commit on new computer
</commit_message>
<xml_diff>
--- a/schedule/index.xlsx
+++ b/schedule/index.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8547" uniqueCount="1494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8547" uniqueCount="1495">
   <si>
     <t>ELECTRICAL AND COMPUTER ENGINEERING</t>
   </si>
@@ -4562,6 +4562,9 @@
   </si>
   <si>
     <t>F 200-340PM</t>
+  </si>
+  <si>
+    <t>Posted 2/15/2019</t>
   </si>
 </sst>
 </file>
@@ -28050,7 +28053,7 @@
       <pane xSplit="1" ySplit="12" topLeftCell="B52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="B64" sqref="B64"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -28066,7 +28069,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="410" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="407" t="s">
-        <v>1113</v>
+        <v>1494</v>
       </c>
       <c r="B1" s="408"/>
       <c r="C1" s="409"/>

</xml_diff>